<commit_message>
Survey processing and time log
</commit_message>
<xml_diff>
--- a/data/processed/User Evaluations/User evaluations-bar charts.xlsx
+++ b/data/processed/User Evaluations/User evaluations-bar charts.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
   <si>
     <t>1. The app always made it clear what the system was currently doing. I could always see where I am on the page and feedback was provided immediately.</t>
   </si>
@@ -60,6 +60,30 @@
   <si>
     <t>10. The app had extra descriptions and help of how to use it if and advice was required.</t>
   </si>
+  <si>
+    <t>Were you able to quickly make a note of how and when you have used a skill in university/workplace etc?</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Num of Participants</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Would you continue to use this app?</t>
+  </si>
+  <si>
+    <t>Did you find the ability to make voice recordings useful?</t>
+  </si>
+  <si>
+    <t>Did you find the statistics page useful?</t>
+  </si>
 </sst>
 </file>
 
@@ -71,18 +95,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4DD0E1"/>
+        <bgColor rgb="FF4DD0E1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -104,14 +137,23 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
     <dxf>
       <font/>
       <fill>
@@ -149,8 +191,28 @@
       </fill>
       <border/>
     </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4DD0E1"/>
+          <bgColor rgb="FF4DD0E1"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE0F7FA"/>
+          <bgColor rgb="FFE0F7FA"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
   </dxfs>
-  <tableStyles count="10">
+  <tableStyles count="14">
     <tableStyle count="3" pivot="0" name="Sheet1-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -162,19 +224,19 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Sheet1-style 3">
-      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="4" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="5" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Sheet1-style 4">
-      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="4" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="5" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Sheet1-style 5">
-      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="4" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+      <tableStyleElement dxfId="5" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="3" pivot="0" name="Sheet1-style 6">
       <tableStyleElement dxfId="1" type="headerRow"/>
@@ -201,6 +263,26 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="Sheet1-style 11">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Sheet1-style 12">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Sheet1-style 13">
+      <tableStyleElement dxfId="4" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="5" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="3" pivot="0" name="Sheet1-style 14">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
@@ -270,11 +352,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1242019365"/>
-        <c:axId val="2038070576"/>
+        <c:axId val="1946228215"/>
+        <c:axId val="1647690597"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1242019365"/>
+        <c:axId val="1946228215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,10 +408,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2038070576"/>
+        <c:crossAx val="1647690597"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2038070576"/>
+        <c:axId val="1647690597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +486,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1242019365"/>
+        <c:crossAx val="1946228215"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -495,11 +577,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="715196852"/>
-        <c:axId val="1234091031"/>
+        <c:axId val="1319042998"/>
+        <c:axId val="696954656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="715196852"/>
+        <c:axId val="1319042998"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,10 +633,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1234091031"/>
+        <c:crossAx val="696954656"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1234091031"/>
+        <c:axId val="696954656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,8 +711,464 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="715196852"/>
+        <c:crossAx val="1319042998"/>
       </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Were you able to quickly make a note of how and when you have used a skill in university/workplace etc?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$103</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$104:$A$105</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$104:$B$105</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Would you continue to use this app?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$111</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$112:$A$113</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$112:$B$113</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Did you find the ability to make voice recordings useful?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$123</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$124:$A$125</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$124:$B$125</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Did you find the statistics page useful?</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$133</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$134:$A$135</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$134:$B$135</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -720,11 +1258,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="621427216"/>
-        <c:axId val="331693801"/>
+        <c:axId val="1889921707"/>
+        <c:axId val="320186084"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="621427216"/>
+        <c:axId val="1889921707"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,10 +1314,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331693801"/>
+        <c:crossAx val="320186084"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331693801"/>
+        <c:axId val="320186084"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +1392,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="621427216"/>
+        <c:crossAx val="1889921707"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -945,11 +1483,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102924068"/>
-        <c:axId val="884109828"/>
+        <c:axId val="786022611"/>
+        <c:axId val="689064184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102924068"/>
+        <c:axId val="786022611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,10 +1539,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="884109828"/>
+        <c:crossAx val="689064184"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="884109828"/>
+        <c:axId val="689064184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1617,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="102924068"/>
+        <c:crossAx val="786022611"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1170,11 +1708,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="766769316"/>
-        <c:axId val="1859189513"/>
+        <c:axId val="642712340"/>
+        <c:axId val="551161238"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="766769316"/>
+        <c:axId val="642712340"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,10 +1764,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1859189513"/>
+        <c:crossAx val="551161238"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1859189513"/>
+        <c:axId val="551161238"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1842,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="766769316"/>
+        <c:crossAx val="642712340"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1395,11 +1933,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2144284786"/>
-        <c:axId val="1178821695"/>
+        <c:axId val="1834109143"/>
+        <c:axId val="1776357990"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144284786"/>
+        <c:axId val="1834109143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,10 +1989,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1178821695"/>
+        <c:crossAx val="1776357990"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1178821695"/>
+        <c:axId val="1776357990"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +2067,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144284786"/>
+        <c:crossAx val="1834109143"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1620,11 +2158,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1817011800"/>
-        <c:axId val="1706012308"/>
+        <c:axId val="1417693852"/>
+        <c:axId val="2042066535"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1817011800"/>
+        <c:axId val="1417693852"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,10 +2214,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1706012308"/>
+        <c:crossAx val="2042066535"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1706012308"/>
+        <c:axId val="2042066535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1754,7 +2292,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1817011800"/>
+        <c:crossAx val="1417693852"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1845,11 +2383,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="719017910"/>
-        <c:axId val="1060339776"/>
+        <c:axId val="908803481"/>
+        <c:axId val="168515521"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="719017910"/>
+        <c:axId val="908803481"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,10 +2439,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1060339776"/>
+        <c:crossAx val="168515521"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1060339776"/>
+        <c:axId val="168515521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +2517,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="719017910"/>
+        <c:crossAx val="908803481"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2070,11 +2608,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="2026043711"/>
-        <c:axId val="1031310530"/>
+        <c:axId val="1228513263"/>
+        <c:axId val="1995231331"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2026043711"/>
+        <c:axId val="1228513263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2126,10 +2664,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1031310530"/>
+        <c:crossAx val="1995231331"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1031310530"/>
+        <c:axId val="1995231331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2742,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2026043711"/>
+        <c:crossAx val="1228513263"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2295,11 +2833,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1737109301"/>
-        <c:axId val="717933224"/>
+        <c:axId val="346625053"/>
+        <c:axId val="992950197"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1737109301"/>
+        <c:axId val="346625053"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,10 +2889,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="717933224"/>
+        <c:crossAx val="992950197"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="717933224"/>
+        <c:axId val="992950197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2429,7 +2967,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1737109301"/>
+        <c:crossAx val="346625053"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2707,11 +3245,111 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4305300" cy="2657475"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 11" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4229100" cy="2619375"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 12" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4229100" cy="2619375"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 13" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4229100" cy="2619375"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 14" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A82:B87" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A72:B77" displayName="Table_1" id="1">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2726,7 +3364,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A52:B57" displayName="Table_10" id="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A22:B27" displayName="Table_10" id="10">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2740,8 +3378,63 @@
 </table>
 </file>
 
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A32:B37" displayName="Table_11" id="11">
+  <tableColumns count="2">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 11" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:B7" displayName="Table_12" id="12">
+  <tableColumns count="2">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 12" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A111:B113" displayName="Table_13" id="13">
+  <tableColumns count="2">
+    <tableColumn name="Response" id="1"/>
+    <tableColumn name="Num of Participants" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 13" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A52:B57" displayName="Table_14" id="14">
+  <tableColumns count="2">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style 14" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A92:B97" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A82:B87" displayName="Table_2" id="2">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2756,52 +3449,37 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A72:B77" displayName="Table_3" id="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A123:B125" displayName="Table_3" id="3">
   <tableColumns count="2">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Response" id="1"/>
+    <tableColumn name="Num of Participants" id="2"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A62:B67" displayName="Table_4" id="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A133:B135" displayName="Table_4" id="4">
   <tableColumns count="2">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Response" id="1"/>
+    <tableColumn name="Num of Participants" id="2"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A12:B17" displayName="Table_5" id="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A103:B105" displayName="Table_5" id="5">
   <tableColumns count="2">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Response" id="1"/>
+    <tableColumn name="Num of Participants" id="2"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style 5" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
-    </ext>
-  </extLst>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A42:B47" displayName="Table_6" id="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A92:B97" displayName="Table_6" id="6">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2816,7 +3494,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A22:B27" displayName="Table_7" id="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A62:B67" displayName="Table_7" id="7">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2831,7 +3509,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A32:B37" displayName="Table_8" id="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A12:B17" displayName="Table_8" id="8">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -2846,7 +3524,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A2:B7" displayName="Table_9" id="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A42:B47" displayName="Table_9" id="9">
   <tableColumns count="2">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
@@ -3120,7 +3798,7 @@
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
@@ -3172,7 +3850,7 @@
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="2"/>
@@ -3224,7 +3902,7 @@
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="2"/>
@@ -3276,7 +3954,7 @@
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="4"/>
+      <c r="B41" s="1"/>
     </row>
     <row r="42">
       <c r="A42" s="2"/>
@@ -3328,7 +4006,7 @@
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B51" s="4"/>
+      <c r="B51" s="1"/>
     </row>
     <row r="52">
       <c r="A52" s="2"/>
@@ -3380,7 +4058,7 @@
       <c r="A61" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B61" s="4"/>
+      <c r="B61" s="1"/>
     </row>
     <row r="62">
       <c r="A62" s="2"/>
@@ -3432,7 +4110,7 @@
       <c r="A71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="4"/>
+      <c r="B71" s="1"/>
     </row>
     <row r="72">
       <c r="A72" s="2"/>
@@ -3484,7 +4162,7 @@
       <c r="A81" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B81" s="4"/>
+      <c r="B81" s="1"/>
     </row>
     <row r="82">
       <c r="A82" s="2"/>
@@ -3536,7 +4214,7 @@
       <c r="A91" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="4"/>
+      <c r="B91" s="1"/>
     </row>
     <row r="92">
       <c r="A92" s="2"/>
@@ -3584,19 +4262,139 @@
         <v>8.0</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B104" s="5">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B105" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B112" s="5">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B113" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B124" s="5">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B125" s="5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B134" s="7">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B135" s="7">
+        <v>1.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
-  <tableParts count="10">
-    <tablePart r:id="rId12"/>
-    <tablePart r:id="rId13"/>
-    <tablePart r:id="rId14"/>
-    <tablePart r:id="rId15"/>
+  <tableParts count="14">
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
     <tablePart r:id="rId18"/>
     <tablePart r:id="rId19"/>
     <tablePart r:id="rId20"/>
     <tablePart r:id="rId21"/>
+    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId24"/>
+    <tablePart r:id="rId25"/>
+    <tablePart r:id="rId26"/>
+    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId28"/>
+    <tablePart r:id="rId29"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>